<commit_message>
committing Albert's changes to online repo
</commit_message>
<xml_diff>
--- a/20211211_Project_management.xlsx
+++ b/20211211_Project_management.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{3A3E0FD2-5253-DC41-9ECC-C167439947E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E150FB-EA5F-854F-B2FB-2357EEED40B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1292,15 +1292,6 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="9" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1311,6 +1302,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1367,6 +1367,36 @@
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
   <dxfs count="31">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1631,36 +1661,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -2027,7 +2027,7 @@
                   <a14:compatExt spid="_x0000_s13313"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001340000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001340000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2058,7 +2058,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0EDB95CA-98FE-4198-8801-690B9B480FDF}" name="Milestones435" displayName="Milestones435" ref="B9:G38" totalsRowShown="0" headerRowDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0EDB95CA-98FE-4198-8801-690B9B480FDF}" name="Milestones435" displayName="Milestones435" ref="B9:G38" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="B9:G38" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2068,9 +2068,9 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6E47A83D-ACD7-4EB6-9B84-5195E813945E}" name="Milestone description" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{529EEF64-D037-4ACF-8CA4-0C10FE2D1FBB}" name="Category" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{711D01BA-2785-403A-9636-CCC7E2ADA584}" name="Assigned to" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{6E47A83D-ACD7-4EB6-9B84-5195E813945E}" name="Milestone description" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{529EEF64-D037-4ACF-8CA4-0C10FE2D1FBB}" name="Category" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{711D01BA-2785-403A-9636-CCC7E2ADA584}" name="Assigned to" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{62B00BEF-16BE-4692-B5E2-F287F680F2C1}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{D6D72902-F68F-4E59-A714-AFFF520C647A}" name="Start" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{93E698DE-286F-49ED-AA20-D0C843671DE8}" name="Days" dataCellStyle="Comma [0]"/>
@@ -2522,8 +2522,8 @@
   </sheetPr>
   <dimension ref="A1:BP40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2544,27 +2544,27 @@
     <row r="1" spans="1:68" ht="25.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:68" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10"/>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="91"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
-      <c r="O2" s="92"/>
-      <c r="P2" s="93"/>
-      <c r="Q2" s="93"/>
-      <c r="R2" s="93"/>
-      <c r="S2" s="93"/>
-      <c r="T2" s="93"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="89"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="90"/>
+      <c r="S2" s="90"/>
+      <c r="T2" s="90"/>
       <c r="U2" s="20"/>
       <c r="V2" s="20"/>
       <c r="W2" s="20"/>
@@ -2691,26 +2691,26 @@
         <v>17</v>
       </c>
       <c r="H4" s="26"/>
-      <c r="I4" s="87" t="s">
+      <c r="I4" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="87"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="87"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
       <c r="M4" s="29"/>
-      <c r="N4" s="88" t="s">
+      <c r="N4" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="O4" s="88"/>
-      <c r="P4" s="88"/>
-      <c r="Q4" s="88"/>
+      <c r="O4" s="92"/>
+      <c r="P4" s="92"/>
+      <c r="Q4" s="92"/>
       <c r="R4" s="29"/>
-      <c r="S4" s="89" t="s">
+      <c r="S4" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="T4" s="89"/>
-      <c r="U4" s="89"/>
-      <c r="V4" s="89"/>
+      <c r="T4" s="93"/>
+      <c r="U4" s="93"/>
+      <c r="V4" s="93"/>
       <c r="W4" s="29"/>
       <c r="X4" s="85" t="s">
         <v>22</v>
@@ -3552,7 +3552,7 @@
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="22">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="F11" s="75">
         <v>44541</v>
@@ -4116,7 +4116,7 @@
         <v>28</v>
       </c>
       <c r="E14" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="75">
         <v>44541</v>
@@ -10032,56 +10032,56 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:BL38">
-    <cfRule type="expression" dxfId="13" priority="7">
+    <cfRule type="expression" dxfId="17" priority="7">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:AM6">
-    <cfRule type="expression" dxfId="12" priority="10">
+    <cfRule type="expression" dxfId="16" priority="10">
       <formula>I$7&lt;=EOMONTH($I$7,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:BL6">
-    <cfRule type="expression" dxfId="11" priority="9">
+    <cfRule type="expression" dxfId="15" priority="9">
       <formula>AND(J$7&lt;=EOMONTH($I$7,2),J$7&gt;EOMONTH($I$7,0),J$7&gt;EOMONTH($I$7,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:BL6">
-    <cfRule type="expression" dxfId="10" priority="8">
+    <cfRule type="expression" dxfId="14" priority="8">
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:BL37">
-    <cfRule type="expression" dxfId="9" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
       <formula>AND($C10="Low Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="14" stopIfTrue="1">
       <formula>AND($C10="High Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="15" stopIfTrue="1">
       <formula>AND($C10="On Track",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="16" stopIfTrue="1">
       <formula>AND($C10="Med Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="17" stopIfTrue="1">
       <formula>AND(LEN($C10)=0,I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38:BL38">
-    <cfRule type="expression" dxfId="4" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="19" stopIfTrue="1">
       <formula>AND(#REF!="Low Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="20" stopIfTrue="1">
       <formula>AND(#REF!="High Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="21" stopIfTrue="1">
       <formula>AND(#REF!="On Track",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="22" stopIfTrue="1">
       <formula>AND(#REF!="Med Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="23" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10234,25 +10234,6 @@
           <xm:sqref>E9:E10 E15:E25 E27:E38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="18" id="{3EF75A3E-8286-4296-914E-C8F63A2E14FB}">
-            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3Flags" iconId="1"/>
-              <x14:cfIcon iconSet="3Signs" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>I38:BL38</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{CFD2A903-1864-0D40-8229-608FE60B5354}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
@@ -10328,6 +10309,25 @@
           <xm:sqref>E11</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="18" id="{3EF75A3E-8286-4296-914E-C8F63A2E14FB}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>I38:BL38</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="53" id="{C84307BC-4E4D-4989-9D21-88D6AEB0AFD2}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -10353,12 +10353,22 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10638,28 +10648,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10686,13 +10690,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update on gantt chart
</commit_message>
<xml_diff>
--- a/20211211_Project_management.xlsx
+++ b/20211211_Project_management.xlsx
@@ -3,19 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E150FB-EA5F-854F-B2FB-2357EEED40B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501461AC-5E1C-D64F-81AD-4F1EA19F2E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="About" sheetId="12" r:id="rId1"/>
-    <sheet name="Dark" sheetId="16" r:id="rId2"/>
+    <sheet name="Dark" sheetId="16" r:id="rId1"/>
+    <sheet name="About" sheetId="12" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">Dark!$6:$9</definedName>
-    <definedName name="Project_Start" localSheetId="1">Dark!$C$6</definedName>
-    <definedName name="Scrolling_Increment" localSheetId="1">Dark!$C$7</definedName>
-    <definedName name="Today" localSheetId="1">TODAY()</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Dark!$6:$9</definedName>
+    <definedName name="Project_Start" localSheetId="0">Dark!$C$6</definedName>
+    <definedName name="Scrolling_Increment" localSheetId="0">Dark!$C$7</definedName>
+    <definedName name="Today" localSheetId="0">TODAY()</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -213,11 +213,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="#,##0_ ;\-#,##0\ "/>
-    <numFmt numFmtId="168" formatCode="d"/>
+    <numFmt numFmtId="166" formatCode="#,##0_ ;\-#,##0\ "/>
+    <numFmt numFmtId="167" formatCode="d"/>
   </numFmts>
   <fonts count="43" x14ac:knownFonts="1">
     <font>
@@ -1009,7 +1009,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
@@ -1021,7 +1021,7 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1102,7 +1102,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1262,22 +1262,22 @@
     <xf numFmtId="14" fontId="0" fillId="10" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="10" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="166" fontId="0" fillId="10" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="12" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="12" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="12" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="12" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="12" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="12" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="12" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="12" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="13" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1360,7 +1360,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Note" xfId="24" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="19" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Per cent" xfId="2" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5" customBuiltin="1"/>
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="26" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="23" builtinId="11" customBuiltin="1"/>
@@ -1946,6 +1946,61 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>25400</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>63500</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>63</xdr:col>
+          <xdr:colOff>228600</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>241300</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="13313" name="Scroll Bar 1" descr="Scroll bar to scroll through the Ghantt project timeline." hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s13313"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001340000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -1999,61 +2054,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>25400</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>63500</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>63</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>241300</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="13313" name="Scroll Bar 1" descr="Scroll bar to scroll through the Ghantt project timeline." hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s13313"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001340000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -2346,184 +2346,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:M19"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="4.6640625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="2.6640625" style="8" customWidth="1"/>
-    <col min="3" max="5" width="40.6640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="7" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="D1" s="61"/>
-    </row>
-    <row r="2" spans="1:13" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-    </row>
-    <row r="3" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="62"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-    </row>
-    <row r="4" spans="1:13" s="8" customFormat="1" ht="67.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="84" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-    </row>
-    <row r="5" spans="1:13" s="8" customFormat="1" ht="67.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="62"/>
-      <c r="C5" s="84" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-    </row>
-    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-    </row>
-    <row r="7" spans="1:13" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-    </row>
-    <row r="8" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-    </row>
-    <row r="9" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="D16" s="8"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="D17" s="8"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="D18" s="8"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="D19" s="8"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-  </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{537EAE25-AFCC-4679-A578-F5918B332482}">
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BP40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A15" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2835,7 +2665,7 @@
       </c>
       <c r="C6" s="33" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">IFERROR(IF(MIN(Milestones435[Start])=0,TODAY(),B15(Milestones435[Start])),TODAY())</f>
-        <v>44541</v>
+        <v>44544</v>
       </c>
       <c r="D6" s="51"/>
       <c r="E6" s="29"/>
@@ -2914,7 +2744,7 @@
       <c r="BE6" s="56"/>
       <c r="BF6" s="56" t="str">
         <f ca="1">IF(OR(TEXT(BF7,"mmmm")=AY6,TEXT(BF7,"mmmm")=AR6,TEXT(BF7,"mmmm")=AK6,TEXT(BF7,"mmmm")=AD6),"",TEXT(BF7,"mmmm"))</f>
-        <v/>
+        <v>February</v>
       </c>
       <c r="BG6" s="56"/>
       <c r="BH6" s="56"/>
@@ -2939,227 +2769,227 @@
       <c r="H7" s="32"/>
       <c r="I7" s="79">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
-        <v>44541</v>
+        <v>44544</v>
       </c>
       <c r="J7" s="80">
         <f ca="1">I7+1</f>
-        <v>44542</v>
+        <v>44545</v>
       </c>
       <c r="K7" s="80">
         <f t="shared" ref="K7:AX7" ca="1" si="0">J7+1</f>
-        <v>44543</v>
+        <v>44546</v>
       </c>
       <c r="L7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44544</v>
+        <v>44547</v>
       </c>
       <c r="M7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44545</v>
+        <v>44548</v>
       </c>
       <c r="N7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44546</v>
+        <v>44549</v>
       </c>
       <c r="O7" s="81">
         <f t="shared" ca="1" si="0"/>
-        <v>44547</v>
+        <v>44550</v>
       </c>
       <c r="P7" s="80">
         <f ca="1">O7+1</f>
-        <v>44548</v>
+        <v>44551</v>
       </c>
       <c r="Q7" s="80">
         <f ca="1">P7+1</f>
-        <v>44549</v>
+        <v>44552</v>
       </c>
       <c r="R7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44550</v>
+        <v>44553</v>
       </c>
       <c r="S7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44551</v>
+        <v>44554</v>
       </c>
       <c r="T7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44552</v>
+        <v>44555</v>
       </c>
       <c r="U7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44553</v>
+        <v>44556</v>
       </c>
       <c r="V7" s="81">
         <f t="shared" ca="1" si="0"/>
-        <v>44554</v>
+        <v>44557</v>
       </c>
       <c r="W7" s="80">
         <f ca="1">V7+1</f>
-        <v>44555</v>
+        <v>44558</v>
       </c>
       <c r="X7" s="80">
         <f ca="1">W7+1</f>
-        <v>44556</v>
+        <v>44559</v>
       </c>
       <c r="Y7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44557</v>
+        <v>44560</v>
       </c>
       <c r="Z7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44558</v>
+        <v>44561</v>
       </c>
       <c r="AA7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44559</v>
+        <v>44562</v>
       </c>
       <c r="AB7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44560</v>
+        <v>44563</v>
       </c>
       <c r="AC7" s="81">
         <f t="shared" ca="1" si="0"/>
-        <v>44561</v>
+        <v>44564</v>
       </c>
       <c r="AD7" s="80">
         <f ca="1">AC7+1</f>
-        <v>44562</v>
+        <v>44565</v>
       </c>
       <c r="AE7" s="80">
         <f ca="1">AD7+1</f>
-        <v>44563</v>
+        <v>44566</v>
       </c>
       <c r="AF7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44564</v>
+        <v>44567</v>
       </c>
       <c r="AG7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44565</v>
+        <v>44568</v>
       </c>
       <c r="AH7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44566</v>
+        <v>44569</v>
       </c>
       <c r="AI7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44567</v>
+        <v>44570</v>
       </c>
       <c r="AJ7" s="81">
         <f t="shared" ca="1" si="0"/>
-        <v>44568</v>
+        <v>44571</v>
       </c>
       <c r="AK7" s="80">
         <f ca="1">AJ7+1</f>
-        <v>44569</v>
+        <v>44572</v>
       </c>
       <c r="AL7" s="80">
         <f ca="1">AK7+1</f>
-        <v>44570</v>
+        <v>44573</v>
       </c>
       <c r="AM7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44571</v>
+        <v>44574</v>
       </c>
       <c r="AN7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44572</v>
+        <v>44575</v>
       </c>
       <c r="AO7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44573</v>
+        <v>44576</v>
       </c>
       <c r="AP7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44574</v>
+        <v>44577</v>
       </c>
       <c r="AQ7" s="81">
         <f t="shared" ca="1" si="0"/>
-        <v>44575</v>
+        <v>44578</v>
       </c>
       <c r="AR7" s="80">
         <f ca="1">AQ7+1</f>
-        <v>44576</v>
+        <v>44579</v>
       </c>
       <c r="AS7" s="80">
         <f ca="1">AR7+1</f>
-        <v>44577</v>
+        <v>44580</v>
       </c>
       <c r="AT7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44578</v>
+        <v>44581</v>
       </c>
       <c r="AU7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44579</v>
+        <v>44582</v>
       </c>
       <c r="AV7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44580</v>
+        <v>44583</v>
       </c>
       <c r="AW7" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>44581</v>
+        <v>44584</v>
       </c>
       <c r="AX7" s="81">
         <f t="shared" ca="1" si="0"/>
-        <v>44582</v>
+        <v>44585</v>
       </c>
       <c r="AY7" s="80">
         <f ca="1">AX7+1</f>
-        <v>44583</v>
+        <v>44586</v>
       </c>
       <c r="AZ7" s="80">
         <f ca="1">AY7+1</f>
-        <v>44584</v>
+        <v>44587</v>
       </c>
       <c r="BA7" s="80">
         <f t="shared" ref="BA7:BE7" ca="1" si="1">AZ7+1</f>
-        <v>44585</v>
+        <v>44588</v>
       </c>
       <c r="BB7" s="80">
         <f t="shared" ca="1" si="1"/>
-        <v>44586</v>
+        <v>44589</v>
       </c>
       <c r="BC7" s="80">
         <f t="shared" ca="1" si="1"/>
-        <v>44587</v>
+        <v>44590</v>
       </c>
       <c r="BD7" s="80">
         <f t="shared" ca="1" si="1"/>
-        <v>44588</v>
+        <v>44591</v>
       </c>
       <c r="BE7" s="81">
         <f t="shared" ca="1" si="1"/>
-        <v>44589</v>
+        <v>44592</v>
       </c>
       <c r="BF7" s="80">
         <f ca="1">BE7+1</f>
-        <v>44590</v>
+        <v>44593</v>
       </c>
       <c r="BG7" s="80">
         <f ca="1">BF7+1</f>
-        <v>44591</v>
+        <v>44594</v>
       </c>
       <c r="BH7" s="80">
         <f t="shared" ref="BH7:BL7" ca="1" si="2">BG7+1</f>
-        <v>44592</v>
+        <v>44595</v>
       </c>
       <c r="BI7" s="80">
         <f t="shared" ca="1" si="2"/>
-        <v>44593</v>
+        <v>44596</v>
       </c>
       <c r="BJ7" s="80">
         <f t="shared" ca="1" si="2"/>
-        <v>44594</v>
+        <v>44597</v>
       </c>
       <c r="BK7" s="80">
         <f t="shared" ca="1" si="2"/>
-        <v>44595</v>
+        <v>44598</v>
       </c>
       <c r="BL7" s="82">
         <f t="shared" ca="1" si="2"/>
-        <v>44596</v>
+        <v>44599</v>
       </c>
       <c r="BM7" s="29"/>
     </row>
@@ -3253,227 +3083,227 @@
       <c r="H9" s="46"/>
       <c r="I9" s="37" t="str">
         <f t="shared" ref="I9:BL9" ca="1" si="3">LEFT(TEXT(I7,"ddd"),1)</f>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="J9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="K9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="L9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="M9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="N9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="O9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="P9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="Q9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="R9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="S9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="T9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="U9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="V9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="W9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="X9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="Y9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="Z9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="AA9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="AB9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AC9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="AD9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AE9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="AF9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="AG9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="AH9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="AI9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AJ9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="AK9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AL9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="AM9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="AN9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="AO9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="AP9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AQ9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="AR9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AS9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="AT9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="AU9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="AV9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="AW9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AX9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="AY9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AZ9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="BA9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="BB9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="BC9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="BD9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="BE9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="BF9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="BG9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="BH9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="BI9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="BJ9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="BK9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="BL9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="BM9" s="29"/>
     </row>
@@ -3879,9 +3709,9 @@
         <v>1</v>
       </c>
       <c r="H13" s="29"/>
-      <c r="I13" s="45">
-        <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+      <c r="I13" s="45" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
       <c r="J13" s="24" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -4125,9 +3955,9 @@
         <v>1</v>
       </c>
       <c r="H14" s="29"/>
-      <c r="I14" s="45">
-        <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+      <c r="I14" s="45" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
       <c r="J14" s="24" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -4605,10 +4435,9 @@
         <v>28</v>
       </c>
       <c r="E16" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="75">
-        <f ca="1">TODAY()</f>
         <v>44541</v>
       </c>
       <c r="G16" s="77">
@@ -4853,10 +4682,10 @@
         <v>30</v>
       </c>
       <c r="E17" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="75">
-        <v>44544</v>
+        <v>44541</v>
       </c>
       <c r="G17" s="77">
         <v>1</v>
@@ -4874,9 +4703,9 @@
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="L17" s="24">
-        <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+      <c r="L17" s="24" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
       <c r="M17" s="24" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -5858,9 +5687,9 @@
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="K21" s="24" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
+      <c r="K21" s="24">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
       </c>
       <c r="L21" s="24" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -5870,9 +5699,9 @@
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="N21" s="24">
-        <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+      <c r="N21" s="24" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
       <c r="O21" s="24" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -7088,9 +6917,9 @@
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="M26" s="24" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
+      <c r="M26" s="24">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
       </c>
       <c r="N26" s="24" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -7100,9 +6929,9 @@
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="P26" s="24">
-        <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+      <c r="P26" s="24" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
       <c r="Q26" s="24" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -7552,10 +7381,10 @@
         <v>0</v>
       </c>
       <c r="F28" s="75">
-        <v>44542</v>
+        <v>44541</v>
       </c>
       <c r="G28" s="77">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H28" s="19"/>
       <c r="I28" s="45" t="str">
@@ -8076,9 +7905,9 @@
         <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
-      <c r="P30" s="24" t="str">
+      <c r="P30" s="24">
         <f t="shared" ca="1" si="13"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="Q30" s="24" t="str">
         <f t="shared" ca="1" si="13"/>
@@ -8088,9 +7917,9 @@
         <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
-      <c r="S30" s="24">
+      <c r="S30" s="24" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="T30" s="24" t="str">
         <f t="shared" ca="1" si="13"/>
@@ -10352,23 +10181,183 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:M19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="2.6640625" style="8" customWidth="1"/>
+    <col min="3" max="5" width="40.6640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="7" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="D1" s="61"/>
+    </row>
+    <row r="2" spans="1:13" ht="50" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+    </row>
+    <row r="3" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+    </row>
+    <row r="4" spans="1:13" s="8" customFormat="1" ht="67.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="84" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+    </row>
+    <row r="5" spans="1:13" s="8" customFormat="1" ht="67.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="84" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+    </row>
+    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="6"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+    </row>
+    <row r="7" spans="1:13" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="D19" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+  </mergeCells>
+  <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10648,22 +10637,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10690,9 +10685,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>